<commit_message>
Adding data from Bloomberg's code
We have the same input as Bloomberg and observe if there is a change in output
</commit_message>
<xml_diff>
--- a/In-Output of Bloomberg's Model/output Bloomberg.xlsx
+++ b/In-Output of Bloomberg's Model/output Bloomberg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Επενδυτική Επιτροπή\BQL files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\Documents\Python_files\Black_Litterman\Iolcus-Investments\In-Output of Bloomberg's Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55D6EE9A-A885-4309-AF2B-2D2C1EDFB58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82515717-4A19-4B15-8280-7FC97E8DBD13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.000000000000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -133,19 +140,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -448,7 +459,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +482,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
       <c r="C2">
@@ -486,7 +497,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>0.41932033957292097</v>
       </c>
       <c r="C3">
@@ -501,7 +512,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>2.580744808016059E-2</v>
       </c>
       <c r="C4">
@@ -516,7 +527,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>2.6562530659644619E-19</v>
       </c>
       <c r="C5">
@@ -531,7 +542,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>0.32626204477625348</v>
       </c>
       <c r="C6">
@@ -546,7 +557,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1.3270126329623039E-3</v>
       </c>
       <c r="C7">
@@ -561,7 +572,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>1.181903836783332E-17</v>
       </c>
       <c r="C8">
@@ -576,7 +587,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>6.6843160067363863E-2</v>
       </c>
       <c r="C9">
@@ -591,7 +602,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>1.9256185836097131E-2</v>
       </c>
       <c r="C10">
@@ -606,7 +617,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>0.1018885487932127</v>
       </c>
       <c r="C11">
@@ -621,7 +632,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>0</v>
       </c>
       <c r="C12">
@@ -636,7 +647,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>3.9295260241028973E-2</v>
       </c>
       <c r="C13">

</xml_diff>